<commit_message>
adjusted mpcs and ran the FIM
</commit_message>
<xml_diff>
--- a/results/01-2024/comparison-deflators-01-2024.xlsx
+++ b/results/01-2024/comparison-deflators-01-2024.xlsx
@@ -815,7 +815,7 @@
         <v>-0.2424</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.2445</v>
+        <v>-0.239</v>
       </c>
       <c r="O5" t="n">
         <v>-0.3884</v>
@@ -1078,40 +1078,40 @@
         <v>-0.0473</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.1022</v>
+        <v>-0.0422</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0362</v>
+        <v>-0.0273</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0236</v>
+        <v>-0.0277</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.026</v>
+        <v>-0.0372</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.0202</v>
+        <v>-0.0357</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.0213</v>
+        <v>-0.0344</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.0296</v>
+        <v>-0.0224</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.0206</v>
+        <v>-0.0152</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.0158</v>
+        <v>-0.0137</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.0108</v>
+        <v>-0.0138</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.0019</v>
+        <v>-0.0129</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.003</v>
+        <v>-0.0143</v>
       </c>
     </row>
     <row r="10">
@@ -1394,64 +1394,64 @@
         <v>23</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3926</v>
+        <v>0.3559</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2349</v>
+        <v>0.1922</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0321</v>
+        <v>0.0208</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0559</v>
+        <v>-0.0658</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.0809</v>
+        <v>-0.1684</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.083</v>
+        <v>-0.1661</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.0507</v>
+        <v>-0.0803</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.0453</v>
+        <v>-0.063</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.505</v>
+        <v>-0.3297</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.5524</v>
+        <v>-0.3425</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.2132</v>
+        <v>-0.1399</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.167</v>
+        <v>-0.1031</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.3077</v>
+        <v>-0.2902</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.2292</v>
+        <v>-0.2613</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.0977</v>
+        <v>-0.1046</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.0289</v>
+        <v>-0.0568</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.0223</v>
+        <v>-0.0915</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.0153</v>
+        <v>-0.0676</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.0073</v>
+        <v>-0.0297</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.0712</v>
+        <v>-0.0777</v>
       </c>
     </row>
     <row r="15">
@@ -1530,64 +1530,64 @@
         <v>23</v>
       </c>
       <c r="C16" t="n">
-        <v>-2.4153</v>
+        <v>-2.452</v>
       </c>
       <c r="D16" t="n">
-        <v>-2.942</v>
+        <v>-2.9847</v>
       </c>
       <c r="E16" t="n">
-        <v>-3.159</v>
+        <v>-3.1702</v>
       </c>
       <c r="F16" t="n">
-        <v>-3.7594</v>
+        <v>-3.7693</v>
       </c>
       <c r="G16" t="n">
-        <v>-4.4973</v>
+        <v>-4.585</v>
       </c>
       <c r="H16" t="n">
-        <v>-2.1663</v>
+        <v>-2.2495</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.4741</v>
+        <v>-0.5037</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1716</v>
+        <v>0.1538</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.3414</v>
+        <v>-0.1066</v>
       </c>
       <c r="L16" t="n">
-        <v>0.4203</v>
+        <v>0.6392</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0984</v>
+        <v>0.1675</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.6786</v>
+        <v>-0.1075</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.5255</v>
+        <v>-0.6267</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.5835</v>
+        <v>-0.7305</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.3406</v>
+        <v>-0.4342</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.5785</v>
+        <v>-0.698</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.4427</v>
+        <v>-0.6044</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.1849</v>
+        <v>-0.2413</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.0103</v>
+        <v>-0.0447</v>
       </c>
       <c r="V16" t="n">
-        <v>-50.1309</v>
+        <v>-50.1495</v>
       </c>
     </row>
     <row r="17">
@@ -1699,7 +1699,7 @@
         <v>-0.2928</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.1239</v>
+        <v>-0.1184</v>
       </c>
       <c r="O18" t="n">
         <v>-0.3653</v>
@@ -1835,31 +1835,31 @@
         <v>-0.012</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.595</v>
+        <v>-0.1125</v>
       </c>
       <c r="O20" t="n">
-        <v>-0.0001</v>
+        <v>-0.1052</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.0001</v>
+        <v>-0.102</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.006</v>
+        <v>-0.0999</v>
       </c>
       <c r="R20" t="n">
-        <v>0</v>
+        <v>-0.0968</v>
       </c>
       <c r="S20" t="n">
-        <v>0</v>
+        <v>-0.0938</v>
       </c>
       <c r="T20" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U20" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="V20" t="n">
-        <v>0</v>
+        <v>-0.0009</v>
       </c>
     </row>
     <row r="21">
@@ -1971,7 +1971,7 @@
         <v>0.503</v>
       </c>
       <c r="N22" t="n">
-        <v>0.0847</v>
+        <v>0.1147</v>
       </c>
       <c r="O22" t="n">
         <v>0.3054</v>
@@ -2243,7 +2243,7 @@
         <v>0.0021</v>
       </c>
       <c r="N26" t="n">
-        <v>0.0082</v>
+        <v>0.0074</v>
       </c>
       <c r="O26" t="n">
         <v>0.0076</v>
@@ -2355,10 +2355,10 @@
         <v>-0.0005</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.0005</v>
+        <v>-0.0006</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.0004</v>
+        <v>-0.0007</v>
       </c>
       <c r="H28" t="n">
         <v>-0.0001</v>
@@ -2367,10 +2367,10 @@
         <v>-0.0001</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.0002</v>
+        <v>-0.0003</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.0004</v>
+        <v>-0.0009</v>
       </c>
       <c r="L28" t="n">
         <v>-0.0001</v>
@@ -2379,25 +2379,25 @@
         <v>-0.0001</v>
       </c>
       <c r="N28" t="n">
-        <v>-0.0015</v>
+        <v>-0.0011</v>
       </c>
       <c r="O28" t="n">
-        <v>-0.0043</v>
+        <v>-0.0025</v>
       </c>
       <c r="P28" t="n">
-        <v>-0.0004</v>
+        <v>-0.0005</v>
       </c>
       <c r="Q28" t="n">
         <v>-0.0004</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.0004</v>
+        <v>-0.0006</v>
       </c>
       <c r="S28" t="n">
-        <v>-0.0004</v>
+        <v>-0.0013</v>
       </c>
       <c r="T28" t="n">
-        <v>-0.0004</v>
+        <v>-0.0003</v>
       </c>
       <c r="U28" t="n">
         <v>-0.0003</v>
@@ -2719,7 +2719,7 @@
         <v>-0.1008</v>
       </c>
       <c r="N33" t="n">
-        <v>0.1308</v>
+        <v>0.1364</v>
       </c>
       <c r="O33" t="n">
         <v>0.0008</v>
@@ -2982,40 +2982,40 @@
         <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>0.009</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>-0.0041</v>
       </c>
       <c r="N37" t="n">
-        <v>0.0001</v>
+        <v>-0.0112</v>
       </c>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>-0.0154</v>
       </c>
       <c r="P37" t="n">
-        <v>0</v>
+        <v>-0.013</v>
       </c>
       <c r="Q37" t="n">
-        <v>0.0001</v>
+        <v>0.0072</v>
       </c>
       <c r="R37" t="n">
-        <v>0</v>
+        <v>0.0055</v>
       </c>
       <c r="S37" t="n">
-        <v>0</v>
+        <v>0.0021</v>
       </c>
       <c r="T37" t="n">
-        <v>0</v>
+        <v>-0.0031</v>
       </c>
       <c r="U37" t="n">
-        <v>0</v>
+        <v>-0.011</v>
       </c>
       <c r="V37" t="n">
-        <v>0</v>
+        <v>-0.0112</v>
       </c>
     </row>
     <row r="38">
@@ -3298,64 +3298,64 @@
         <v>51</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>-0.0366</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>-0.0427</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>-0.0112</v>
       </c>
       <c r="F42" t="n">
-        <v>0</v>
+        <v>-0.0099</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>-0.0875</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>-0.0831</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>-0.0295</v>
       </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>-0.0177</v>
       </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>0.1753</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>0.2099</v>
       </c>
       <c r="M42" t="n">
-        <v>0.0113</v>
+        <v>0.0845</v>
       </c>
       <c r="N42" t="n">
-        <v>0.0088</v>
+        <v>0.0728</v>
       </c>
       <c r="O42" t="n">
-        <v>0.0085</v>
+        <v>0.0261</v>
       </c>
       <c r="P42" t="n">
-        <v>0.0078</v>
+        <v>-0.0243</v>
       </c>
       <c r="Q42" t="n">
-        <v>0.0069</v>
+        <v>0.0001</v>
       </c>
       <c r="R42" t="n">
-        <v>0.0067</v>
+        <v>-0.0213</v>
       </c>
       <c r="S42" t="n">
-        <v>0.0065</v>
+        <v>-0.0626</v>
       </c>
       <c r="T42" t="n">
-        <v>0.0064</v>
+        <v>-0.0459</v>
       </c>
       <c r="U42" t="n">
-        <v>0.0057</v>
+        <v>-0.0167</v>
       </c>
       <c r="V42" t="n">
-        <v>-0.0033</v>
+        <v>-0.0097</v>
       </c>
     </row>
     <row r="43">
@@ -3434,64 +3434,64 @@
         <v>51</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>-0.0366</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>-0.0427</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>-0.0112</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>-0.0099</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>-0.0878</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>-0.0831</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>-0.0295</v>
       </c>
       <c r="J44" t="n">
-        <v>0</v>
+        <v>-0.0178</v>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
+        <v>0.2348</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>0.2189</v>
       </c>
       <c r="M44" t="n">
-        <v>0.3778</v>
+        <v>0.4469</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0127</v>
+        <v>0.5838</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0191</v>
+        <v>-0.0821</v>
       </c>
       <c r="P44" t="n">
-        <v>0.0283</v>
+        <v>-0.1187</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.0149</v>
+        <v>-0.0787</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.0238</v>
+        <v>-0.1434</v>
       </c>
       <c r="S44" t="n">
-        <v>-0.0119</v>
+        <v>-0.1737</v>
       </c>
       <c r="T44" t="n">
-        <v>-0.0132</v>
+        <v>-0.0696</v>
       </c>
       <c r="U44" t="n">
-        <v>-0.0079</v>
+        <v>-0.0423</v>
       </c>
       <c r="V44" t="n">
-        <v>0.0993</v>
+        <v>0.0807</v>
       </c>
     </row>
     <row r="45">
@@ -3603,7 +3603,7 @@
         <v>-0.2449</v>
       </c>
       <c r="N46" t="n">
-        <v>0.1315</v>
+        <v>0.1371</v>
       </c>
       <c r="O46" t="n">
         <v>0.001</v>
@@ -3739,31 +3739,31 @@
         <v>0</v>
       </c>
       <c r="N48" t="n">
-        <v>0.0011</v>
+        <v>0.4836</v>
       </c>
       <c r="O48" t="n">
-        <v>0</v>
+        <v>-0.105</v>
       </c>
       <c r="P48" t="n">
-        <v>0</v>
+        <v>-0.1019</v>
       </c>
       <c r="Q48" t="n">
-        <v>0</v>
+        <v>-0.0939</v>
       </c>
       <c r="R48" t="n">
-        <v>0</v>
+        <v>-0.0968</v>
       </c>
       <c r="S48" t="n">
-        <v>0</v>
+        <v>-0.0938</v>
       </c>
       <c r="T48" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="U48" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="V48" t="n">
-        <v>0</v>
+        <v>-0.0009</v>
       </c>
     </row>
     <row r="49">
@@ -3875,7 +3875,7 @@
         <v>0.471</v>
       </c>
       <c r="N50" t="n">
-        <v>-0.1315</v>
+        <v>-0.1015</v>
       </c>
       <c r="O50" t="n">
         <v>-0.0008</v>
@@ -4147,7 +4147,7 @@
         <v>-0.0054</v>
       </c>
       <c r="N54" t="n">
-        <v>0</v>
+        <v>-0.0008</v>
       </c>
       <c r="O54" t="n">
         <v>0</v>
@@ -4259,10 +4259,10 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="G56" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -4271,10 +4271,10 @@
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="K56" t="n">
-        <v>0</v>
+        <v>-0.0005</v>
       </c>
       <c r="L56" t="n">
         <v>0</v>
@@ -4283,10 +4283,10 @@
         <v>0.0005</v>
       </c>
       <c r="N56" t="n">
-        <v>-0.0001</v>
+        <v>0.0004</v>
       </c>
       <c r="O56" t="n">
-        <v>0</v>
+        <v>0.0018</v>
       </c>
       <c r="P56" t="n">
         <v>0</v>
@@ -4295,10 +4295,10 @@
         <v>0</v>
       </c>
       <c r="R56" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="S56" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="T56" t="n">
         <v>0</v>
@@ -4307,7 +4307,7 @@
         <v>0</v>
       </c>
       <c r="V56" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="57">

</xml_diff>